<commit_message>
tested with apache poi 5.0.0
</commit_message>
<xml_diff>
--- a/apache-poi-excel-text-alignment/excel-text-alignment.xlsx
+++ b/apache-poi-excel-text-alignment/excel-text-alignment.xlsx
@@ -62,16 +62,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment wrapText="true" horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment wrapText="true" horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment wrapText="true" horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment wrapText="true" horizontal="center"/>
     </xf>
   </cellXfs>

</xml_diff>